<commit_message>
Added date to the excel sheet
</commit_message>
<xml_diff>
--- a/MASTER_TEMPLATE.xlsx
+++ b/MASTER_TEMPLATE.xlsx
@@ -868,12 +868,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -885,6 +879,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
@@ -1574,8 +1574,8 @@
   </sheetPr>
   <dimension ref="A1:AML64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -9868,14 +9868,14 @@
     </row>
     <row r="10" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="30"/>
-      <c r="B10" s="69" t="s">
+      <c r="B10" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="69"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="76"/>
       <c r="H10" s="18" t="s">
         <v>38</v>
       </c>
@@ -10899,12 +10899,12 @@
     </row>
     <row r="11" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23"/>
-      <c r="B11" s="69"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="69"/>
-      <c r="G11" s="69"/>
+      <c r="B11" s="76"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="76"/>
       <c r="H11" s="14" t="s">
         <v>39</v>
       </c>
@@ -11930,12 +11930,12 @@
     </row>
     <row r="12" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23"/>
-      <c r="B12" s="69"/>
-      <c r="C12" s="69"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="69"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="69"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
       <c r="H12" s="18" t="s">
         <v>22</v>
       </c>
@@ -12960,12 +12960,12 @@
     </row>
     <row r="13" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23"/>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="69"/>
+      <c r="B13" s="76"/>
+      <c r="C13" s="76"/>
+      <c r="D13" s="76"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="76"/>
       <c r="H13" s="19" t="s">
         <v>23</v>
       </c>
@@ -13991,12 +13991,12 @@
     </row>
     <row r="14" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="23"/>
-      <c r="B14" s="69"/>
-      <c r="C14" s="69"/>
-      <c r="D14" s="69"/>
-      <c r="E14" s="69"/>
-      <c r="F14" s="69"/>
-      <c r="G14" s="69"/>
+      <c r="B14" s="76"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="76"/>
       <c r="H14" s="19" t="s">
         <v>20</v>
       </c>
@@ -15022,12 +15022,12 @@
     </row>
     <row r="15" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="23"/>
-      <c r="B15" s="69"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="69"/>
-      <c r="G15" s="69"/>
+      <c r="B15" s="76"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76"/>
       <c r="H15" s="19"/>
       <c r="I15" s="45"/>
       <c r="J15" s="25"/>
@@ -18129,7 +18129,7 @@
       <c r="D19" s="35"/>
       <c r="E19" s="35"/>
       <c r="F19" s="35"/>
-      <c r="G19" s="73"/>
+      <c r="G19" s="71"/>
       <c r="H19" s="25"/>
       <c r="I19" s="43"/>
       <c r="J19" s="59"/>
@@ -19151,30 +19151,30 @@
     </row>
     <row r="20" spans="1:1025" s="12" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="13"/>
-      <c r="B20" s="74"/>
-      <c r="C20" s="74"/>
-      <c r="D20" s="74"/>
-      <c r="E20" s="74"/>
-      <c r="F20" s="74"/>
-      <c r="G20" s="74"/>
+      <c r="B20" s="72"/>
+      <c r="C20" s="72"/>
+      <c r="D20" s="72"/>
+      <c r="E20" s="72"/>
+      <c r="F20" s="72"/>
+      <c r="G20" s="72"/>
       <c r="I20" s="46"/>
     </row>
     <row r="21" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="30"/>
-      <c r="B21" s="75" t="s">
+      <c r="B21" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="75"/>
-      <c r="D21" s="75"/>
-      <c r="E21" s="75" t="s">
+      <c r="C21" s="73"/>
+      <c r="D21" s="73"/>
+      <c r="E21" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="F21" s="75"/>
-      <c r="G21" s="75"/>
-      <c r="H21" s="70"/>
-      <c r="I21" s="71"/>
-      <c r="J21" s="72"/>
-      <c r="K21" s="72"/>
+      <c r="F21" s="73"/>
+      <c r="G21" s="73"/>
+      <c r="H21" s="68"/>
+      <c r="I21" s="69"/>
+      <c r="J21" s="70"/>
+      <c r="K21" s="70"/>
       <c r="L21" s="59"/>
       <c r="M21" s="59"/>
       <c r="N21" s="59"/>
@@ -20192,12 +20192,12 @@
     </row>
     <row r="22" spans="1:1025" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="22"/>
-      <c r="B22" s="76"/>
-      <c r="C22" s="76"/>
-      <c r="D22" s="76"/>
-      <c r="E22" s="76"/>
-      <c r="F22" s="76"/>
-      <c r="G22" s="76"/>
+      <c r="B22" s="74"/>
+      <c r="C22" s="74"/>
+      <c r="D22" s="74"/>
+      <c r="E22" s="74"/>
+      <c r="F22" s="74"/>
+      <c r="G22" s="74"/>
       <c r="H22" s="21"/>
       <c r="I22" s="48"/>
       <c r="J22" s="59"/>
@@ -30510,14 +30510,14 @@
     </row>
     <row r="32" spans="1:1025" s="12" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="13"/>
-      <c r="B32" s="68" t="s">
+      <c r="B32" s="75" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="68"/>
-      <c r="D32" s="68"/>
-      <c r="E32" s="68"/>
-      <c r="F32" s="68"/>
-      <c r="G32" s="68"/>
+      <c r="C32" s="75"/>
+      <c r="D32" s="75"/>
+      <c r="E32" s="75"/>
+      <c r="F32" s="75"/>
+      <c r="G32" s="75"/>
       <c r="H32" s="40" t="s">
         <v>40</v>
       </c>
@@ -30525,12 +30525,12 @@
     </row>
     <row r="33" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="57"/>
-      <c r="B33" s="68"/>
-      <c r="C33" s="68"/>
-      <c r="D33" s="68"/>
-      <c r="E33" s="68"/>
-      <c r="F33" s="68"/>
-      <c r="G33" s="68"/>
+      <c r="B33" s="75"/>
+      <c r="C33" s="75"/>
+      <c r="D33" s="75"/>
+      <c r="E33" s="75"/>
+      <c r="F33" s="75"/>
+      <c r="G33" s="75"/>
       <c r="H33" s="50" t="s">
         <v>45</v>
       </c>
@@ -31556,12 +31556,12 @@
     </row>
     <row r="34" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="57"/>
-      <c r="B34" s="68"/>
-      <c r="C34" s="68"/>
-      <c r="D34" s="68"/>
-      <c r="E34" s="68"/>
-      <c r="F34" s="68"/>
-      <c r="G34" s="68"/>
+      <c r="B34" s="75"/>
+      <c r="C34" s="75"/>
+      <c r="D34" s="75"/>
+      <c r="E34" s="75"/>
+      <c r="F34" s="75"/>
+      <c r="G34" s="75"/>
       <c r="H34" s="50" t="s">
         <v>46</v>
       </c>
@@ -32587,12 +32587,12 @@
     </row>
     <row r="35" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="57"/>
-      <c r="B35" s="68"/>
-      <c r="C35" s="68"/>
-      <c r="D35" s="68"/>
-      <c r="E35" s="68"/>
-      <c r="F35" s="68"/>
-      <c r="G35" s="68"/>
+      <c r="B35" s="75"/>
+      <c r="C35" s="75"/>
+      <c r="D35" s="75"/>
+      <c r="E35" s="75"/>
+      <c r="F35" s="75"/>
+      <c r="G35" s="75"/>
       <c r="H35" s="50" t="s">
         <v>47</v>
       </c>
@@ -33618,12 +33618,12 @@
     </row>
     <row r="36" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="57"/>
-      <c r="B36" s="68"/>
-      <c r="C36" s="68"/>
-      <c r="D36" s="68"/>
-      <c r="E36" s="68"/>
-      <c r="F36" s="68"/>
-      <c r="G36" s="68"/>
+      <c r="B36" s="75"/>
+      <c r="C36" s="75"/>
+      <c r="D36" s="75"/>
+      <c r="E36" s="75"/>
+      <c r="F36" s="75"/>
+      <c r="G36" s="75"/>
       <c r="H36" s="50" t="s">
         <v>48</v>
       </c>
@@ -34649,12 +34649,12 @@
     </row>
     <row r="37" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="57"/>
-      <c r="B37" s="68"/>
-      <c r="C37" s="68"/>
-      <c r="D37" s="68"/>
-      <c r="E37" s="68"/>
-      <c r="F37" s="68"/>
-      <c r="G37" s="68"/>
+      <c r="B37" s="75"/>
+      <c r="C37" s="75"/>
+      <c r="D37" s="75"/>
+      <c r="E37" s="75"/>
+      <c r="F37" s="75"/>
+      <c r="G37" s="75"/>
       <c r="H37" s="50" t="s">
         <v>50</v>
       </c>
@@ -35680,12 +35680,12 @@
     </row>
     <row r="38" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="57"/>
-      <c r="B38" s="68"/>
-      <c r="C38" s="68"/>
-      <c r="D38" s="68"/>
-      <c r="E38" s="68"/>
-      <c r="F38" s="68"/>
-      <c r="G38" s="68"/>
+      <c r="B38" s="75"/>
+      <c r="C38" s="75"/>
+      <c r="D38" s="75"/>
+      <c r="E38" s="75"/>
+      <c r="F38" s="75"/>
+      <c r="G38" s="75"/>
       <c r="H38" s="40"/>
       <c r="I38" s="56"/>
       <c r="J38" s="59"/>

</xml_diff>

<commit_message>
Finished the formatting fix for the excel sheets
A macro is added to MASTER_TEMPLATE that runs when the spreadsheet opens if the cell K2 contains 0
Fixed a bug with converting the string to a number
Added macro flag to the xlsm file
</commit_message>
<xml_diff>
--- a/MASTER_TEMPLATE.xlsx
+++ b/MASTER_TEMPLATE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="8232"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="8235"/>
   </bookViews>
   <sheets>
     <sheet name="100Hr 15April2015 " sheetId="1" r:id="rId1"/>
@@ -451,7 +451,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -591,6 +591,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -699,7 +705,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -884,6 +890,10 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1575,20 +1585,20 @@
   <dimension ref="A1:AML64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="1" style="14" customWidth="1"/>
-    <col min="2" max="7" width="14.77734375" style="14" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" style="14" customWidth="1"/>
-    <col min="9" max="9" width="7.44140625" style="54" customWidth="1"/>
-    <col min="10" max="1026" width="9.109375" style="14"/>
-    <col min="1027" max="16384" width="8.88671875" style="59"/>
+    <col min="2" max="7" width="14.7109375" style="14" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" style="14" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" style="54" customWidth="1"/>
+    <col min="10" max="1026" width="9.140625" style="14" customWidth="1"/>
+    <col min="1027" max="16384" width="8.85546875" style="59"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -2621,7 +2631,7 @@
       <c r="AMJ1" s="59"/>
       <c r="AMK1" s="59"/>
     </row>
-    <row r="2" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
@@ -3656,7 +3666,7 @@
       <c r="AMJ2" s="59"/>
       <c r="AMK2" s="59"/>
     </row>
-    <row r="3" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
       <c r="C3" s="10"/>
@@ -4689,7 +4699,7 @@
       <c r="AMJ3" s="59"/>
       <c r="AMK3" s="59"/>
     </row>
-    <row r="4" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="7"/>
       <c r="C4" s="11"/>
@@ -5722,7 +5732,7 @@
       <c r="AMJ4" s="59"/>
       <c r="AMK4" s="59"/>
     </row>
-    <row r="5" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="34"/>
       <c r="B5" s="35"/>
       <c r="C5" s="35"/>
@@ -6753,7 +6763,7 @@
       <c r="AMJ5" s="59"/>
       <c r="AMK5" s="59"/>
     </row>
-    <row r="6" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="30"/>
       <c r="B6" s="32" t="s">
         <v>25</v>
@@ -7786,7 +7796,7 @@
       <c r="AMJ6" s="59"/>
       <c r="AMK6" s="59"/>
     </row>
-    <row r="7" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="30"/>
       <c r="B7" s="32" t="s">
         <v>26</v>
@@ -8820,7 +8830,7 @@
       <c r="AMJ7" s="59"/>
       <c r="AMK7" s="59"/>
     </row>
-    <row r="8" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="30"/>
       <c r="B8" s="32" t="s">
         <v>35</v>
@@ -9849,7 +9859,7 @@
       <c r="AMJ8" s="59"/>
       <c r="AMK8" s="59"/>
     </row>
-    <row r="9" spans="1:1025" s="12" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1025" s="12" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13"/>
       <c r="B9" s="35" t="s">
         <v>36</v>
@@ -9866,7 +9876,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="30"/>
       <c r="B10" s="76" t="s">
         <v>37</v>
@@ -10897,7 +10907,7 @@
       <c r="AMJ10" s="59"/>
       <c r="AMK10" s="59"/>
     </row>
-    <row r="11" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="23"/>
       <c r="B11" s="76"/>
       <c r="C11" s="76"/>
@@ -10905,7 +10915,7 @@
       <c r="E11" s="76"/>
       <c r="F11" s="76"/>
       <c r="G11" s="76"/>
-      <c r="H11" s="14" t="s">
+      <c r="H11" s="77" t="s">
         <v>39</v>
       </c>
       <c r="I11" s="44">
@@ -11928,7 +11938,7 @@
       <c r="AMJ11" s="59"/>
       <c r="AMK11" s="59"/>
     </row>
-    <row r="12" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="23"/>
       <c r="B12" s="76"/>
       <c r="C12" s="76"/>
@@ -12958,7 +12968,7 @@
       <c r="AMJ12" s="59"/>
       <c r="AMK12" s="59"/>
     </row>
-    <row r="13" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="23"/>
       <c r="B13" s="76"/>
       <c r="C13" s="76"/>
@@ -13989,7 +13999,7 @@
       <c r="AMJ13" s="59"/>
       <c r="AMK13" s="59"/>
     </row>
-    <row r="14" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="23"/>
       <c r="B14" s="76"/>
       <c r="C14" s="76"/>
@@ -15020,7 +15030,7 @@
       <c r="AMJ14" s="59"/>
       <c r="AMK14" s="59"/>
     </row>
-    <row r="15" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="23"/>
       <c r="B15" s="76"/>
       <c r="C15" s="76"/>
@@ -16041,7 +16051,7 @@
       <c r="AMJ15" s="59"/>
       <c r="AMK15" s="59"/>
     </row>
-    <row r="16" spans="1:1025" s="25" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1025" s="25" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="24"/>
       <c r="B16" s="32" t="s">
         <v>28</v>
@@ -16062,7 +16072,7 @@
       <c r="Q16" s="26"/>
       <c r="R16" s="26"/>
     </row>
-    <row r="17" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="30"/>
       <c r="B17" s="32" t="s">
         <v>29</v>
@@ -17091,7 +17101,7 @@
       <c r="AMJ17" s="59"/>
       <c r="AMK17" s="59"/>
     </row>
-    <row r="18" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="30"/>
       <c r="B18" s="35" t="s">
         <v>27</v>
@@ -18122,7 +18132,7 @@
       <c r="AMJ18" s="59"/>
       <c r="AMK18" s="59"/>
     </row>
-    <row r="19" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="31"/>
       <c r="B19" s="35"/>
       <c r="C19" s="35"/>
@@ -19149,7 +19159,7 @@
       <c r="AMJ19" s="59"/>
       <c r="AMK19" s="59"/>
     </row>
-    <row r="20" spans="1:1025" s="12" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:1025" s="12" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="13"/>
       <c r="B20" s="72"/>
       <c r="C20" s="72"/>
@@ -19159,7 +19169,7 @@
       <c r="G20" s="72"/>
       <c r="I20" s="46"/>
     </row>
-    <row r="21" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="30"/>
       <c r="B21" s="73" t="s">
         <v>52</v>
@@ -20190,7 +20200,7 @@
       <c r="AMJ21" s="59"/>
       <c r="AMK21" s="59"/>
     </row>
-    <row r="22" spans="1:1025" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1025" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="22"/>
       <c r="B22" s="74"/>
       <c r="C22" s="74"/>
@@ -21217,7 +21227,7 @@
       <c r="AMJ22" s="59"/>
       <c r="AMK22" s="59"/>
     </row>
-    <row r="23" spans="1:1025" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1025" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="59"/>
       <c r="B23" s="59"/>
       <c r="C23" s="59"/>
@@ -22244,7 +22254,7 @@
       <c r="AMJ23" s="59"/>
       <c r="AMK23" s="59"/>
     </row>
-    <row r="24" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="C24" s="3"/>
@@ -23279,7 +23289,7 @@
       <c r="AMJ24" s="59"/>
       <c r="AMK24" s="59"/>
     </row>
-    <row r="25" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
@@ -24316,7 +24326,7 @@
       <c r="AMJ25" s="59"/>
       <c r="AMK25" s="59"/>
     </row>
-    <row r="26" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="B26" s="7"/>
       <c r="C26" s="10"/>
@@ -25349,7 +25359,7 @@
       <c r="AMJ26" s="59"/>
       <c r="AMK26" s="59"/>
     </row>
-    <row r="27" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
       <c r="B27" s="7"/>
       <c r="C27" s="11"/>
@@ -26382,7 +26392,7 @@
       <c r="AMJ27" s="59"/>
       <c r="AMK27" s="59"/>
     </row>
-    <row r="28" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="34"/>
       <c r="B28" s="35"/>
       <c r="C28" s="35"/>
@@ -27413,7 +27423,7 @@
       <c r="AMJ28" s="59"/>
       <c r="AMK28" s="59"/>
     </row>
-    <row r="29" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="30"/>
       <c r="B29" s="32" t="s">
         <v>17</v>
@@ -28446,7 +28456,7 @@
       <c r="AMJ29" s="59"/>
       <c r="AMK29" s="59"/>
     </row>
-    <row r="30" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="30"/>
       <c r="B30" s="32" t="s">
         <v>13</v>
@@ -29480,7 +29490,7 @@
       <c r="AMJ30" s="59"/>
       <c r="AMK30" s="59"/>
     </row>
-    <row r="31" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="30"/>
       <c r="B31" s="32" t="s">
         <v>9</v>
@@ -30508,7 +30518,7 @@
       <c r="AMJ31" s="59"/>
       <c r="AMK31" s="59"/>
     </row>
-    <row r="32" spans="1:1025" s="12" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:1025" s="12" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="13"/>
       <c r="B32" s="75" t="s">
         <v>49</v>
@@ -30523,7 +30533,7 @@
       </c>
       <c r="I32" s="56"/>
     </row>
-    <row r="33" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="57"/>
       <c r="B33" s="75"/>
       <c r="C33" s="75"/>
@@ -31554,7 +31564,7 @@
       <c r="AMJ33" s="59"/>
       <c r="AMK33" s="59"/>
     </row>
-    <row r="34" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="57"/>
       <c r="B34" s="75"/>
       <c r="C34" s="75"/>
@@ -32585,7 +32595,7 @@
       <c r="AMJ34" s="59"/>
       <c r="AMK34" s="59"/>
     </row>
-    <row r="35" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="57"/>
       <c r="B35" s="75"/>
       <c r="C35" s="75"/>
@@ -33616,7 +33626,7 @@
       <c r="AMJ35" s="59"/>
       <c r="AMK35" s="59"/>
     </row>
-    <row r="36" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="57"/>
       <c r="B36" s="75"/>
       <c r="C36" s="75"/>
@@ -34647,7 +34657,7 @@
       <c r="AMJ36" s="59"/>
       <c r="AMK36" s="59"/>
     </row>
-    <row r="37" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="57"/>
       <c r="B37" s="75"/>
       <c r="C37" s="75"/>
@@ -34658,7 +34668,7 @@
       <c r="H37" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="I37" s="58">
+      <c r="I37" s="78">
         <v>9531.4</v>
       </c>
       <c r="J37" s="59"/>
@@ -35678,7 +35688,7 @@
       <c r="AMJ37" s="59"/>
       <c r="AMK37" s="59"/>
     </row>
-    <row r="38" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="57"/>
       <c r="B38" s="75"/>
       <c r="C38" s="75"/>
@@ -36705,7 +36715,7 @@
       <c r="AMJ38" s="59"/>
       <c r="AMK38" s="59"/>
     </row>
-    <row r="39" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="30"/>
       <c r="B39" s="35" t="s">
         <v>10</v>
@@ -37734,14 +37744,14 @@
       <c r="AMJ39" s="59"/>
       <c r="AMK39" s="59"/>
     </row>
-    <row r="40" spans="1:1025" s="25" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1025" s="25" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="24"/>
       <c r="B40" s="25" t="s">
         <v>32</v>
       </c>
       <c r="I40" s="43"/>
     </row>
-    <row r="41" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="30"/>
       <c r="B41" s="32" t="s">
         <v>11</v>
@@ -38773,7 +38783,7 @@
       <c r="AMJ41" s="59"/>
       <c r="AMK41" s="59"/>
     </row>
-    <row r="42" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="31"/>
       <c r="B42" s="32"/>
       <c r="C42" s="32"/>
@@ -39799,11 +39809,11 @@
       <c r="AMJ42" s="59"/>
       <c r="AMK42" s="59"/>
     </row>
-    <row r="43" spans="1:1025" s="12" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:1025" s="12" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="13"/>
       <c r="I43" s="46"/>
     </row>
-    <row r="44" spans="1:1025" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="27"/>
       <c r="B44" s="52" t="str">
         <f>B21</f>
@@ -40836,7 +40846,7 @@
       <c r="AMJ44" s="59"/>
       <c r="AMK44" s="59"/>
     </row>
-    <row r="45" spans="1:1025" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1025" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="22"/>
       <c r="B45" s="21"/>
       <c r="C45" s="21"/>
@@ -41863,7 +41873,7 @@
       <c r="AMJ45" s="59"/>
       <c r="AMK45" s="59"/>
     </row>
-    <row r="46" spans="1:1025" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1025" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="59"/>
       <c r="B46" s="59"/>
       <c r="C46" s="59"/>
@@ -42890,7 +42900,7 @@
       <c r="AMJ46" s="59"/>
       <c r="AMK46" s="59"/>
     </row>
-    <row r="47" spans="1:1025" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="C47" s="3"/>
@@ -43925,7 +43935,7 @@
       <c r="AMJ47" s="59"/>
       <c r="AMK47" s="59"/>
     </row>
-    <row r="48" spans="1:1025" ht="13.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="B48" s="7"/>
       <c r="C48" s="8"/>
@@ -44962,7 +44972,7 @@
       <c r="AMJ48" s="59"/>
       <c r="AMK48" s="59"/>
     </row>
-    <row r="49" spans="1:1025" ht="13.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="6"/>
       <c r="B49" s="7"/>
       <c r="C49" s="10"/>
@@ -45995,7 +46005,7 @@
       <c r="AMJ49" s="59"/>
       <c r="AMK49" s="59"/>
     </row>
-    <row r="50" spans="1:1025" ht="13.05" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="6"/>
       <c r="B50" s="7"/>
       <c r="C50" s="11"/>
@@ -47028,7 +47038,7 @@
       <c r="AMJ50" s="59"/>
       <c r="AMK50" s="59"/>
     </row>
-    <row r="51" spans="1:1025" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="34"/>
       <c r="B51" s="35"/>
       <c r="C51" s="35"/>
@@ -48059,7 +48069,7 @@
       <c r="AMJ51" s="59"/>
       <c r="AMK51" s="59"/>
     </row>
-    <row r="52" spans="1:1025" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="30"/>
       <c r="B52" s="32" t="s">
         <v>30</v>
@@ -49093,7 +49103,7 @@
       <c r="AMJ52" s="59"/>
       <c r="AMK52" s="59"/>
     </row>
-    <row r="53" spans="1:1025" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="30"/>
       <c r="B53" s="32" t="s">
         <v>31</v>
@@ -50127,7 +50137,7 @@
       <c r="AMJ53" s="59"/>
       <c r="AMK53" s="59"/>
     </row>
-    <row r="54" spans="1:1025" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="34"/>
       <c r="B54" s="35"/>
       <c r="C54" s="35"/>
@@ -51153,7 +51163,7 @@
       <c r="AMJ54" s="59"/>
       <c r="AMK54" s="59"/>
     </row>
-    <row r="55" spans="1:1025" s="12" customFormat="1" ht="13.05" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:1025" s="12" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="13"/>
       <c r="B55" s="38" t="s">
         <v>12</v>
@@ -51166,7 +51176,7 @@
       <c r="H55" s="38"/>
       <c r="I55" s="49"/>
     </row>
-    <row r="56" spans="1:1025" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="37"/>
       <c r="B56" s="38"/>
       <c r="C56" s="38"/>
@@ -52193,7 +52203,7 @@
       <c r="AMJ56" s="59"/>
       <c r="AMK56" s="59"/>
     </row>
-    <row r="57" spans="1:1025" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="30"/>
       <c r="B57" s="35" t="s">
         <v>33</v>
@@ -53222,7 +53232,7 @@
       <c r="AMJ57" s="59"/>
       <c r="AMK57" s="59"/>
     </row>
-    <row r="58" spans="1:1025" s="25" customFormat="1" ht="13.05" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1025" s="25" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="24"/>
       <c r="B58" s="35" t="s">
         <v>34</v>
@@ -53237,7 +53247,7 @@
       </c>
       <c r="I58" s="43"/>
     </row>
-    <row r="59" spans="1:1025" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="31"/>
       <c r="B59" s="32"/>
       <c r="C59" s="32"/>
@@ -54264,7 +54274,7 @@
       <c r="AMJ59" s="59"/>
       <c r="AMK59" s="59"/>
     </row>
-    <row r="60" spans="1:1025" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="31"/>
       <c r="B60" s="32"/>
       <c r="C60" s="32"/>
@@ -55290,11 +55300,11 @@
       <c r="AMJ60" s="59"/>
       <c r="AMK60" s="59"/>
     </row>
-    <row r="61" spans="1:1025" s="12" customFormat="1" ht="13.05" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:1025" s="12" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="13"/>
       <c r="I61" s="46"/>
     </row>
-    <row r="62" spans="1:1025" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1025" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="27"/>
       <c r="B62" s="53" t="str">
         <f>B21</f>
@@ -55311,7 +55321,7 @@
       <c r="H62" s="33"/>
       <c r="I62" s="47"/>
     </row>
-    <row r="63" spans="1:1025" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1025" x14ac:dyDescent="0.2">
       <c r="A63" s="63"/>
       <c r="B63" s="55"/>
       <c r="C63" s="55"/>
@@ -55322,7 +55332,7 @@
       <c r="H63" s="55"/>
       <c r="I63" s="64"/>
     </row>
-    <row r="64" spans="1:1025" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1025" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="65"/>
       <c r="B64" s="66"/>
       <c r="C64" s="66"/>
@@ -55352,7 +55362,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>